<commit_message>
se hace cambios de excel de registro de empleados
</commit_message>
<xml_diff>
--- a/src/Views/assets/excel/paciente_registro.xlsx
+++ b/src/Views/assets/excel/paciente_registro.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t xml:space="preserve">Relacion de Solicitudes</t>
+    <t xml:space="preserve">Registro de Pacientes</t>
   </si>
   <si>
     <t>#</t>
@@ -30,7 +30,7 @@
     <t xml:space="preserve">N° Identificacion</t>
   </si>
   <si>
-    <t>Dieta</t>
+    <t>Torre</t>
   </si>
   <si>
     <t>Cama</t>

</xml_diff>

<commit_message>
se coloca un selecct en registrar paciente
</commit_message>
<xml_diff>
--- a/src/Views/assets/excel/paciente_registro.xlsx
+++ b/src/Views/assets/excel/paciente_registro.xlsx
@@ -884,6 +884,7 @@
       <c r="M8" s="2"/>
     </row>
     <row r="9" ht="14.25">
+      <c r="D9" s="10"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -894,6 +895,7 @@
       <c r="M9" s="2"/>
     </row>
     <row r="10" ht="14.25">
+      <c r="D10" s="10"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -904,6 +906,7 @@
       <c r="M10" s="2"/>
     </row>
     <row r="11" ht="14.25">
+      <c r="D11" s="10"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -914,6 +917,7 @@
       <c r="M11" s="2"/>
     </row>
     <row r="12" ht="14.25">
+      <c r="D12" s="10"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -924,6 +928,7 @@
       <c r="M12" s="2"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
+      <c r="D13" s="10"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -935,6 +940,7 @@
       <c r="M13" s="2"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
+      <c r="D14" s="10"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -946,6 +952,7 @@
       <c r="M14" s="2"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
+      <c r="D15" s="10"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -957,25 +964,80 @@
       <c r="M15" s="2"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
+      <c r="D16" s="10"/>
       <c r="E16" s="2"/>
     </row>
     <row r="17" ht="14.25" customHeight="1">
+      <c r="D17" s="10"/>
       <c r="E17" s="2"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
+      <c r="D18" s="10"/>
       <c r="E18" s="2"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
+      <c r="D19" s="10"/>
       <c r="E19" s="2"/>
     </row>
     <row r="20" ht="14.25" customHeight="1">
+      <c r="D20" s="10"/>
       <c r="E20" s="2"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
+      <c r="D21" s="10"/>
       <c r="E21" s="2"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
+      <c r="D22" s="10"/>
       <c r="E22" s="2"/>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="D23" s="10"/>
+    </row>
+    <row r="24" ht="14.25">
+      <c r="D24" s="10"/>
+    </row>
+    <row r="25" ht="14.25">
+      <c r="D25" s="10"/>
+    </row>
+    <row r="26" ht="14.25">
+      <c r="D26" s="10"/>
+    </row>
+    <row r="27" ht="14.25">
+      <c r="D27" s="10"/>
+    </row>
+    <row r="28" ht="14.25">
+      <c r="D28" s="10"/>
+    </row>
+    <row r="29" ht="14.25">
+      <c r="D29" s="10"/>
+    </row>
+    <row r="30" ht="14.25">
+      <c r="D30" s="10"/>
+    </row>
+    <row r="31" ht="14.25">
+      <c r="D31" s="10"/>
+    </row>
+    <row r="32" ht="14.25">
+      <c r="D32" s="10"/>
+    </row>
+    <row r="33" ht="14.25">
+      <c r="D33" s="10"/>
+    </row>
+    <row r="34" ht="14.25">
+      <c r="D34" s="10"/>
+    </row>
+    <row r="35" ht="14.25">
+      <c r="D35" s="10"/>
+    </row>
+    <row r="36" ht="14.25">
+      <c r="D36" s="10"/>
+    </row>
+    <row r="37" ht="14.25">
+      <c r="D37" s="10"/>
+    </row>
+    <row r="38" ht="14.25">
+      <c r="D38" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -986,5 +1048,23 @@
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
+        <x14:dataValidation xr:uid="{00A000D9-0035-4356-813D-003300B90040}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>$H$3:$I$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>H3:I3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00B9001C-002C-4DC6-8D5F-00F9002000B3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>$H$3:$I$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>D3 D4 D5 D6 D7 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D22 D23 D24 D25 D26 D27 D28 D29 D30 D31 D32 D33 D34 D35 D36 D37 D38</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>